<commit_message>
updated analysis. added wastewater
</commit_message>
<xml_diff>
--- a/santa_clara_county/FOIA_data_request_kirsch_analysis.xlsx
+++ b/santa_clara_county/FOIA_data_request_kirsch_analysis.xlsx
@@ -3,18 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8F6B10-D79C-4B78-88E4-C988A42CC2D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275C3F76-2BDA-4C43-B910-903927E1A626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12" yWindow="366" windowWidth="23028" windowHeight="12078" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="by Quarter" sheetId="3" r:id="rId1"/>
-    <sheet name="conclusions" sheetId="5" r:id="rId2"/>
-    <sheet name="all-cause deaths" sheetId="1" r:id="rId3"/>
-    <sheet name="covid deaths by quarter" sheetId="4" r:id="rId4"/>
-    <sheet name="covid deaths" sheetId="2" r:id="rId5"/>
+    <sheet name="conclusions" sheetId="5" r:id="rId1"/>
+    <sheet name="by Quarter" sheetId="3" r:id="rId2"/>
+    <sheet name="cases in LTCF" sheetId="6" r:id="rId3"/>
+    <sheet name="all-cause deaths" sheetId="1" r:id="rId4"/>
+    <sheet name="covid deaths by quarter" sheetId="4" r:id="rId5"/>
+    <sheet name="covid deaths" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="4" r:id="rId7"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="65">
   <si>
     <t>age_group</t>
   </si>
@@ -192,6 +196,42 @@
   <si>
     <t>CACM</t>
   </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Sum of New_cases</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>Qtr1</t>
+  </si>
+  <si>
+    <t>Qtr2</t>
+  </si>
+  <si>
+    <t>Qtr3</t>
+  </si>
+  <si>
+    <t>Qtr4</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Linked to source</t>
+  </si>
+  <si>
+    <t>local values only copy</t>
+  </si>
+  <si>
+    <t>NCACM % inncrease of Q1 2021 vs. Q1 2020</t>
+  </si>
 </sst>
 </file>
 
@@ -242,10 +282,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5609,6 +5656,152 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>11430</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C757BD61-29FD-A98C-EB2C-D99CF684FBAB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="739140" y="377190"/>
+          <a:ext cx="10439400" cy="4004310"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>Q1 2021</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t> vs Q1 2020 is shows a large statistically significant increase in non-COVID NCACM. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t>It was 66% for those in their 60s an 30% for those in their 70s.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t>It wasn't COVID since these are NOT covid deaths. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t>the question of the Q4 2020 COVID deaths vs. Q1 2021 COVID deaths depends on COVID cases. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t>Earlier analysis showed the CFR increased. But this </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t>there are two ways to validate the COVID cases:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t>1. the actual reported cases in LTCFs</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t>2. the wastewater </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>25</xdr:col>
       <xdr:colOff>762000</xdr:colOff>
       <xdr:row>0</xdr:row>
@@ -5682,114 +5875,2815 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>99060</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C757BD61-29FD-A98C-EB2C-D99CF684FBAB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="739140" y="304800"/>
-          <a:ext cx="10439400" cy="4076700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" kern="1200"/>
-            <a:t>Q1 2021</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" kern="1200" baseline="0"/>
-            <a:t> vs Q1 2020 is HIGHLY statistically significant increase in NCACM (30%)</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100" kern="1200" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" kern="1200" baseline="0"/>
-            <a:t>the question of the Q4 2020 COVID deaths vs. Q1 2021 COVID deaths depends on COVID cases.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100" kern="1200" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" kern="1200" baseline="0"/>
-            <a:t>there are two ways to esimate the COVID cases:</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" kern="1200" baseline="0"/>
-            <a:t>1. the actual reported cases in LTCFs</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" kern="1200" baseline="0"/>
-            <a:t>2. the wasewater</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Author" refreshedDate="45612.629074189812" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="376" xr:uid="{F2FD9A7A-8820-4EED-8159-25ACCA9C5CA0}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:C377" sheet="COVID-19_cases_at_Long_Term_Car" r:id="rId2"/>
+  </cacheSource>
+  <cacheFields count="6">
+    <cacheField name="New_cases" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="173"/>
+    </cacheField>
+    <cacheField name="Total_cases" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="6393"/>
+    </cacheField>
+    <cacheField name="Date" numFmtId="14">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2020-02-24T00:00:00" maxDate="2021-05-06T00:00:00" count="376">
+        <d v="2020-02-24T00:00:00"/>
+        <d v="2020-03-04T00:00:00"/>
+        <d v="2020-03-06T00:00:00"/>
+        <d v="2020-03-07T00:00:00"/>
+        <d v="2020-03-08T00:00:00"/>
+        <d v="2020-03-09T00:00:00"/>
+        <d v="2020-03-10T00:00:00"/>
+        <d v="2020-03-11T00:00:00"/>
+        <d v="2020-03-12T00:00:00"/>
+        <d v="2020-03-13T00:00:00"/>
+        <d v="2020-03-14T00:00:00"/>
+        <d v="2020-03-15T00:00:00"/>
+        <d v="2020-03-17T00:00:00"/>
+        <d v="2020-03-18T00:00:00"/>
+        <d v="2020-03-20T00:00:00"/>
+        <d v="2020-03-21T00:00:00"/>
+        <d v="2020-03-22T00:00:00"/>
+        <d v="2020-03-23T00:00:00"/>
+        <d v="2020-03-24T00:00:00"/>
+        <d v="2020-03-25T00:00:00"/>
+        <d v="2020-03-26T00:00:00"/>
+        <d v="2020-03-27T00:00:00"/>
+        <d v="2020-03-28T00:00:00"/>
+        <d v="2020-03-29T00:00:00"/>
+        <d v="2020-03-30T00:00:00"/>
+        <d v="2020-03-31T00:00:00"/>
+        <d v="2020-04-01T00:00:00"/>
+        <d v="2020-04-02T00:00:00"/>
+        <d v="2020-04-03T00:00:00"/>
+        <d v="2020-04-04T00:00:00"/>
+        <d v="2020-04-05T00:00:00"/>
+        <d v="2020-04-06T00:00:00"/>
+        <d v="2020-04-07T00:00:00"/>
+        <d v="2020-04-08T00:00:00"/>
+        <d v="2020-04-09T00:00:00"/>
+        <d v="2020-04-10T00:00:00"/>
+        <d v="2020-04-11T00:00:00"/>
+        <d v="2020-04-12T00:00:00"/>
+        <d v="2020-04-13T00:00:00"/>
+        <d v="2020-04-14T00:00:00"/>
+        <d v="2020-04-15T00:00:00"/>
+        <d v="2020-04-16T00:00:00"/>
+        <d v="2020-04-17T00:00:00"/>
+        <d v="2020-04-18T00:00:00"/>
+        <d v="2020-04-19T00:00:00"/>
+        <d v="2020-04-20T00:00:00"/>
+        <d v="2020-04-21T00:00:00"/>
+        <d v="2020-04-22T00:00:00"/>
+        <d v="2020-04-23T00:00:00"/>
+        <d v="2020-04-24T00:00:00"/>
+        <d v="2020-04-25T00:00:00"/>
+        <d v="2020-04-26T00:00:00"/>
+        <d v="2020-04-27T00:00:00"/>
+        <d v="2020-04-28T00:00:00"/>
+        <d v="2020-04-29T00:00:00"/>
+        <d v="2020-04-30T00:00:00"/>
+        <d v="2020-05-01T00:00:00"/>
+        <d v="2020-05-02T00:00:00"/>
+        <d v="2020-05-03T00:00:00"/>
+        <d v="2020-05-04T00:00:00"/>
+        <d v="2020-05-05T00:00:00"/>
+        <d v="2020-05-06T00:00:00"/>
+        <d v="2020-05-07T00:00:00"/>
+        <d v="2020-05-08T00:00:00"/>
+        <d v="2020-05-09T00:00:00"/>
+        <d v="2020-05-10T00:00:00"/>
+        <d v="2020-05-11T00:00:00"/>
+        <d v="2020-05-13T00:00:00"/>
+        <d v="2020-05-16T00:00:00"/>
+        <d v="2020-05-18T00:00:00"/>
+        <d v="2020-05-19T00:00:00"/>
+        <d v="2020-05-20T00:00:00"/>
+        <d v="2020-05-21T00:00:00"/>
+        <d v="2020-05-22T00:00:00"/>
+        <d v="2020-05-26T00:00:00"/>
+        <d v="2020-05-27T00:00:00"/>
+        <d v="2020-05-28T00:00:00"/>
+        <d v="2020-05-29T00:00:00"/>
+        <d v="2020-05-30T00:00:00"/>
+        <d v="2020-06-01T00:00:00"/>
+        <d v="2020-06-02T00:00:00"/>
+        <d v="2020-06-03T00:00:00"/>
+        <d v="2020-06-04T00:00:00"/>
+        <d v="2020-06-05T00:00:00"/>
+        <d v="2020-06-06T00:00:00"/>
+        <d v="2020-06-07T00:00:00"/>
+        <d v="2020-06-08T00:00:00"/>
+        <d v="2020-06-09T00:00:00"/>
+        <d v="2020-06-10T00:00:00"/>
+        <d v="2020-06-11T00:00:00"/>
+        <d v="2020-06-12T00:00:00"/>
+        <d v="2020-06-13T00:00:00"/>
+        <d v="2020-06-14T00:00:00"/>
+        <d v="2020-06-15T00:00:00"/>
+        <d v="2020-06-16T00:00:00"/>
+        <d v="2020-06-17T00:00:00"/>
+        <d v="2020-06-18T00:00:00"/>
+        <d v="2020-06-19T00:00:00"/>
+        <d v="2020-06-20T00:00:00"/>
+        <d v="2020-06-21T00:00:00"/>
+        <d v="2020-06-22T00:00:00"/>
+        <d v="2020-06-23T00:00:00"/>
+        <d v="2020-06-24T00:00:00"/>
+        <d v="2020-06-25T00:00:00"/>
+        <d v="2020-06-26T00:00:00"/>
+        <d v="2020-06-27T00:00:00"/>
+        <d v="2020-06-28T00:00:00"/>
+        <d v="2020-06-29T00:00:00"/>
+        <d v="2020-06-30T00:00:00"/>
+        <d v="2020-07-01T00:00:00"/>
+        <d v="2020-07-03T00:00:00"/>
+        <d v="2020-07-04T00:00:00"/>
+        <d v="2020-07-05T00:00:00"/>
+        <d v="2020-07-06T00:00:00"/>
+        <d v="2020-07-07T00:00:00"/>
+        <d v="2020-07-08T00:00:00"/>
+        <d v="2020-07-09T00:00:00"/>
+        <d v="2020-07-10T00:00:00"/>
+        <d v="2020-07-11T00:00:00"/>
+        <d v="2020-07-12T00:00:00"/>
+        <d v="2020-07-13T00:00:00"/>
+        <d v="2020-07-14T00:00:00"/>
+        <d v="2020-07-15T00:00:00"/>
+        <d v="2020-07-16T00:00:00"/>
+        <d v="2020-07-17T00:00:00"/>
+        <d v="2020-07-18T00:00:00"/>
+        <d v="2020-07-19T00:00:00"/>
+        <d v="2020-07-20T00:00:00"/>
+        <d v="2020-07-21T00:00:00"/>
+        <d v="2020-07-22T00:00:00"/>
+        <d v="2020-07-23T00:00:00"/>
+        <d v="2020-07-24T00:00:00"/>
+        <d v="2020-07-25T00:00:00"/>
+        <d v="2020-07-26T00:00:00"/>
+        <d v="2020-07-27T00:00:00"/>
+        <d v="2020-07-28T00:00:00"/>
+        <d v="2020-07-29T00:00:00"/>
+        <d v="2020-07-30T00:00:00"/>
+        <d v="2020-07-31T00:00:00"/>
+        <d v="2020-08-01T00:00:00"/>
+        <d v="2020-08-02T00:00:00"/>
+        <d v="2020-08-03T00:00:00"/>
+        <d v="2020-08-04T00:00:00"/>
+        <d v="2020-08-05T00:00:00"/>
+        <d v="2020-08-06T00:00:00"/>
+        <d v="2020-08-07T00:00:00"/>
+        <d v="2020-08-08T00:00:00"/>
+        <d v="2020-08-09T00:00:00"/>
+        <d v="2020-08-10T00:00:00"/>
+        <d v="2020-08-11T00:00:00"/>
+        <d v="2020-08-12T00:00:00"/>
+        <d v="2020-08-13T00:00:00"/>
+        <d v="2020-08-14T00:00:00"/>
+        <d v="2020-08-15T00:00:00"/>
+        <d v="2020-08-16T00:00:00"/>
+        <d v="2020-08-17T00:00:00"/>
+        <d v="2020-08-18T00:00:00"/>
+        <d v="2020-08-19T00:00:00"/>
+        <d v="2020-08-20T00:00:00"/>
+        <d v="2020-08-21T00:00:00"/>
+        <d v="2020-08-22T00:00:00"/>
+        <d v="2020-08-23T00:00:00"/>
+        <d v="2020-08-24T00:00:00"/>
+        <d v="2020-08-25T00:00:00"/>
+        <d v="2020-08-26T00:00:00"/>
+        <d v="2020-08-27T00:00:00"/>
+        <d v="2020-08-28T00:00:00"/>
+        <d v="2020-08-29T00:00:00"/>
+        <d v="2020-08-30T00:00:00"/>
+        <d v="2020-08-31T00:00:00"/>
+        <d v="2020-09-01T00:00:00"/>
+        <d v="2020-09-02T00:00:00"/>
+        <d v="2020-09-03T00:00:00"/>
+        <d v="2020-09-04T00:00:00"/>
+        <d v="2020-09-05T00:00:00"/>
+        <d v="2020-09-06T00:00:00"/>
+        <d v="2020-09-07T00:00:00"/>
+        <d v="2020-09-08T00:00:00"/>
+        <d v="2020-09-09T00:00:00"/>
+        <d v="2020-09-10T00:00:00"/>
+        <d v="2020-09-12T00:00:00"/>
+        <d v="2020-09-13T00:00:00"/>
+        <d v="2020-09-14T00:00:00"/>
+        <d v="2020-09-15T00:00:00"/>
+        <d v="2020-09-16T00:00:00"/>
+        <d v="2020-09-17T00:00:00"/>
+        <d v="2020-09-18T00:00:00"/>
+        <d v="2020-09-19T00:00:00"/>
+        <d v="2020-09-20T00:00:00"/>
+        <d v="2020-09-21T00:00:00"/>
+        <d v="2020-09-22T00:00:00"/>
+        <d v="2020-09-23T00:00:00"/>
+        <d v="2020-09-24T00:00:00"/>
+        <d v="2020-09-25T00:00:00"/>
+        <d v="2020-09-26T00:00:00"/>
+        <d v="2020-09-27T00:00:00"/>
+        <d v="2020-09-28T00:00:00"/>
+        <d v="2020-09-29T00:00:00"/>
+        <d v="2020-09-30T00:00:00"/>
+        <d v="2020-10-01T00:00:00"/>
+        <d v="2020-10-02T00:00:00"/>
+        <d v="2020-10-03T00:00:00"/>
+        <d v="2020-10-04T00:00:00"/>
+        <d v="2020-10-05T00:00:00"/>
+        <d v="2020-10-06T00:00:00"/>
+        <d v="2020-10-07T00:00:00"/>
+        <d v="2020-10-08T00:00:00"/>
+        <d v="2020-10-09T00:00:00"/>
+        <d v="2020-10-10T00:00:00"/>
+        <d v="2020-10-11T00:00:00"/>
+        <d v="2020-10-12T00:00:00"/>
+        <d v="2020-10-13T00:00:00"/>
+        <d v="2020-10-14T00:00:00"/>
+        <d v="2020-10-15T00:00:00"/>
+        <d v="2020-10-16T00:00:00"/>
+        <d v="2020-10-17T00:00:00"/>
+        <d v="2020-10-18T00:00:00"/>
+        <d v="2020-10-19T00:00:00"/>
+        <d v="2020-10-20T00:00:00"/>
+        <d v="2020-10-21T00:00:00"/>
+        <d v="2020-10-22T00:00:00"/>
+        <d v="2020-10-23T00:00:00"/>
+        <d v="2020-10-24T00:00:00"/>
+        <d v="2020-10-26T00:00:00"/>
+        <d v="2020-10-27T00:00:00"/>
+        <d v="2020-10-28T00:00:00"/>
+        <d v="2020-10-29T00:00:00"/>
+        <d v="2020-10-30T00:00:00"/>
+        <d v="2020-10-31T00:00:00"/>
+        <d v="2020-11-01T00:00:00"/>
+        <d v="2020-11-02T00:00:00"/>
+        <d v="2020-11-03T00:00:00"/>
+        <d v="2020-11-04T00:00:00"/>
+        <d v="2020-11-05T00:00:00"/>
+        <d v="2020-11-06T00:00:00"/>
+        <d v="2020-11-07T00:00:00"/>
+        <d v="2020-11-08T00:00:00"/>
+        <d v="2020-11-09T00:00:00"/>
+        <d v="2020-11-10T00:00:00"/>
+        <d v="2020-11-11T00:00:00"/>
+        <d v="2020-11-12T00:00:00"/>
+        <d v="2020-11-13T00:00:00"/>
+        <d v="2020-11-14T00:00:00"/>
+        <d v="2020-11-15T00:00:00"/>
+        <d v="2020-11-16T00:00:00"/>
+        <d v="2020-11-17T00:00:00"/>
+        <d v="2020-11-18T00:00:00"/>
+        <d v="2020-11-19T00:00:00"/>
+        <d v="2020-11-20T00:00:00"/>
+        <d v="2020-11-21T00:00:00"/>
+        <d v="2020-11-22T00:00:00"/>
+        <d v="2020-11-23T00:00:00"/>
+        <d v="2020-11-24T00:00:00"/>
+        <d v="2020-11-25T00:00:00"/>
+        <d v="2020-11-26T00:00:00"/>
+        <d v="2020-11-27T00:00:00"/>
+        <d v="2020-11-28T00:00:00"/>
+        <d v="2020-11-29T00:00:00"/>
+        <d v="2020-11-30T00:00:00"/>
+        <d v="2020-12-01T00:00:00"/>
+        <d v="2020-12-02T00:00:00"/>
+        <d v="2020-12-03T00:00:00"/>
+        <d v="2020-12-04T00:00:00"/>
+        <d v="2020-12-05T00:00:00"/>
+        <d v="2020-12-06T00:00:00"/>
+        <d v="2020-12-07T00:00:00"/>
+        <d v="2020-12-08T00:00:00"/>
+        <d v="2020-12-09T00:00:00"/>
+        <d v="2020-12-10T00:00:00"/>
+        <d v="2020-12-11T00:00:00"/>
+        <d v="2020-12-12T00:00:00"/>
+        <d v="2020-12-13T00:00:00"/>
+        <d v="2020-12-14T00:00:00"/>
+        <d v="2020-12-15T00:00:00"/>
+        <d v="2020-12-16T00:00:00"/>
+        <d v="2020-12-17T00:00:00"/>
+        <d v="2020-12-18T00:00:00"/>
+        <d v="2020-12-19T00:00:00"/>
+        <d v="2020-12-20T00:00:00"/>
+        <d v="2020-12-21T00:00:00"/>
+        <d v="2020-12-22T00:00:00"/>
+        <d v="2020-12-23T00:00:00"/>
+        <d v="2020-12-24T00:00:00"/>
+        <d v="2020-12-25T00:00:00"/>
+        <d v="2020-12-26T00:00:00"/>
+        <d v="2020-12-27T00:00:00"/>
+        <d v="2020-12-28T00:00:00"/>
+        <d v="2020-12-29T00:00:00"/>
+        <d v="2020-12-30T00:00:00"/>
+        <d v="2020-12-31T00:00:00"/>
+        <d v="2021-01-01T00:00:00"/>
+        <d v="2021-01-02T00:00:00"/>
+        <d v="2021-01-03T00:00:00"/>
+        <d v="2021-01-04T00:00:00"/>
+        <d v="2021-01-05T00:00:00"/>
+        <d v="2021-01-06T00:00:00"/>
+        <d v="2021-01-07T00:00:00"/>
+        <d v="2021-01-08T00:00:00"/>
+        <d v="2021-01-09T00:00:00"/>
+        <d v="2021-01-10T00:00:00"/>
+        <d v="2021-01-11T00:00:00"/>
+        <d v="2021-01-12T00:00:00"/>
+        <d v="2021-01-13T00:00:00"/>
+        <d v="2021-01-14T00:00:00"/>
+        <d v="2021-01-15T00:00:00"/>
+        <d v="2021-01-16T00:00:00"/>
+        <d v="2021-01-17T00:00:00"/>
+        <d v="2021-01-18T00:00:00"/>
+        <d v="2021-01-19T00:00:00"/>
+        <d v="2021-01-20T00:00:00"/>
+        <d v="2021-01-21T00:00:00"/>
+        <d v="2021-01-22T00:00:00"/>
+        <d v="2021-01-23T00:00:00"/>
+        <d v="2021-01-24T00:00:00"/>
+        <d v="2021-01-25T00:00:00"/>
+        <d v="2021-01-26T00:00:00"/>
+        <d v="2021-01-27T00:00:00"/>
+        <d v="2021-01-28T00:00:00"/>
+        <d v="2021-01-29T00:00:00"/>
+        <d v="2021-01-30T00:00:00"/>
+        <d v="2021-01-31T00:00:00"/>
+        <d v="2021-02-01T00:00:00"/>
+        <d v="2021-02-02T00:00:00"/>
+        <d v="2021-02-03T00:00:00"/>
+        <d v="2021-02-04T00:00:00"/>
+        <d v="2021-02-05T00:00:00"/>
+        <d v="2021-02-06T00:00:00"/>
+        <d v="2021-02-07T00:00:00"/>
+        <d v="2021-02-08T00:00:00"/>
+        <d v="2021-02-09T00:00:00"/>
+        <d v="2021-02-10T00:00:00"/>
+        <d v="2021-02-11T00:00:00"/>
+        <d v="2021-02-12T00:00:00"/>
+        <d v="2021-02-13T00:00:00"/>
+        <d v="2021-02-15T00:00:00"/>
+        <d v="2021-02-17T00:00:00"/>
+        <d v="2021-02-18T00:00:00"/>
+        <d v="2021-02-19T00:00:00"/>
+        <d v="2021-02-20T00:00:00"/>
+        <d v="2021-02-21T00:00:00"/>
+        <d v="2021-02-22T00:00:00"/>
+        <d v="2021-02-23T00:00:00"/>
+        <d v="2021-02-24T00:00:00"/>
+        <d v="2021-02-26T00:00:00"/>
+        <d v="2021-02-28T00:00:00"/>
+        <d v="2021-03-01T00:00:00"/>
+        <d v="2021-03-08T00:00:00"/>
+        <d v="2021-03-10T00:00:00"/>
+        <d v="2021-03-11T00:00:00"/>
+        <d v="2021-03-12T00:00:00"/>
+        <d v="2021-03-13T00:00:00"/>
+        <d v="2021-03-14T00:00:00"/>
+        <d v="2021-03-15T00:00:00"/>
+        <d v="2021-03-23T00:00:00"/>
+        <d v="2021-03-26T00:00:00"/>
+        <d v="2021-03-27T00:00:00"/>
+        <d v="2021-03-30T00:00:00"/>
+        <d v="2021-03-31T00:00:00"/>
+        <d v="2021-04-01T00:00:00"/>
+        <d v="2021-04-04T00:00:00"/>
+        <d v="2021-04-05T00:00:00"/>
+        <d v="2021-04-06T00:00:00"/>
+        <d v="2021-04-07T00:00:00"/>
+        <d v="2021-04-09T00:00:00"/>
+        <d v="2021-04-10T00:00:00"/>
+        <d v="2021-04-13T00:00:00"/>
+        <d v="2021-04-15T00:00:00"/>
+        <d v="2021-04-19T00:00:00"/>
+        <d v="2021-04-21T00:00:00"/>
+        <d v="2021-04-22T00:00:00"/>
+        <d v="2021-04-26T00:00:00"/>
+        <d v="2021-04-27T00:00:00"/>
+        <d v="2021-04-28T00:00:00"/>
+        <d v="2021-04-29T00:00:00"/>
+        <d v="2021-05-03T00:00:00"/>
+        <d v="2021-05-05T00:00:00"/>
+      </sharedItems>
+      <fieldGroup par="5"/>
+    </cacheField>
+    <cacheField name="Months (Date)" numFmtId="0" databaseField="0">
+      <fieldGroup base="2">
+        <rangePr groupBy="months" startDate="2020-02-24T00:00:00" endDate="2021-05-06T00:00:00"/>
+        <groupItems count="14">
+          <s v="&lt;2/24/2020"/>
+          <s v="Jan"/>
+          <s v="Feb"/>
+          <s v="Mar"/>
+          <s v="Apr"/>
+          <s v="May"/>
+          <s v="Jun"/>
+          <s v="Jul"/>
+          <s v="Aug"/>
+          <s v="Sep"/>
+          <s v="Oct"/>
+          <s v="Nov"/>
+          <s v="Dec"/>
+          <s v="&gt;5/6/2021"/>
+        </groupItems>
+      </fieldGroup>
+    </cacheField>
+    <cacheField name="Quarters (Date)" numFmtId="0" databaseField="0">
+      <fieldGroup base="2">
+        <rangePr groupBy="quarters" startDate="2020-02-24T00:00:00" endDate="2021-05-06T00:00:00"/>
+        <groupItems count="6">
+          <s v="&lt;2/24/2020"/>
+          <s v="Qtr1"/>
+          <s v="Qtr2"/>
+          <s v="Qtr3"/>
+          <s v="Qtr4"/>
+          <s v="&gt;5/6/2021"/>
+        </groupItems>
+      </fieldGroup>
+    </cacheField>
+    <cacheField name="Years (Date)" numFmtId="0" databaseField="0">
+      <fieldGroup base="2">
+        <rangePr groupBy="years" startDate="2020-02-24T00:00:00" endDate="2021-05-06T00:00:00"/>
+        <groupItems count="4">
+          <s v="&lt;2/24/2020"/>
+          <s v="2020"/>
+          <s v="2021"/>
+          <s v="&gt;5/6/2021"/>
+        </groupItems>
+      </fieldGroup>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="376">
+  <r>
+    <n v="1"/>
+    <n v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="4"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="5"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="7"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="9"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <n v="12"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="13"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="14"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <n v="17"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="18"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="20"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="22"/>
+    <x v="12"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <n v="27"/>
+    <x v="13"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="31"/>
+    <x v="14"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="32"/>
+    <x v="15"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <n v="35"/>
+    <x v="16"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <n v="38"/>
+    <x v="17"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="42"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <n v="50"/>
+    <x v="19"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <n v="57"/>
+    <x v="20"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <n v="63"/>
+    <x v="21"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <n v="69"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <n v="75"/>
+    <x v="23"/>
+  </r>
+  <r>
+    <n v="17"/>
+    <n v="92"/>
+    <x v="24"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <n v="101"/>
+    <x v="25"/>
+  </r>
+  <r>
+    <n v="16"/>
+    <n v="117"/>
+    <x v="26"/>
+  </r>
+  <r>
+    <n v="13"/>
+    <n v="130"/>
+    <x v="27"/>
+  </r>
+  <r>
+    <n v="22"/>
+    <n v="152"/>
+    <x v="28"/>
+  </r>
+  <r>
+    <n v="15"/>
+    <n v="167"/>
+    <x v="29"/>
+  </r>
+  <r>
+    <n v="17"/>
+    <n v="184"/>
+    <x v="30"/>
+  </r>
+  <r>
+    <n v="17"/>
+    <n v="201"/>
+    <x v="31"/>
+  </r>
+  <r>
+    <n v="29"/>
+    <n v="230"/>
+    <x v="32"/>
+  </r>
+  <r>
+    <n v="45"/>
+    <n v="275"/>
+    <x v="33"/>
+  </r>
+  <r>
+    <n v="25"/>
+    <n v="300"/>
+    <x v="34"/>
+  </r>
+  <r>
+    <n v="26"/>
+    <n v="326"/>
+    <x v="35"/>
+  </r>
+  <r>
+    <n v="31"/>
+    <n v="357"/>
+    <x v="36"/>
+  </r>
+  <r>
+    <n v="25"/>
+    <n v="382"/>
+    <x v="37"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <n v="390"/>
+    <x v="38"/>
+  </r>
+  <r>
+    <n v="17"/>
+    <n v="407"/>
+    <x v="39"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="411"/>
+    <x v="40"/>
+  </r>
+  <r>
+    <n v="14"/>
+    <n v="425"/>
+    <x v="41"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <n v="431"/>
+    <x v="42"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <n v="437"/>
+    <x v="43"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <n v="442"/>
+    <x v="44"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <n v="449"/>
+    <x v="45"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <n v="455"/>
+    <x v="46"/>
+  </r>
+  <r>
+    <n v="24"/>
+    <n v="479"/>
+    <x v="47"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="481"/>
+    <x v="48"/>
+  </r>
+  <r>
+    <n v="15"/>
+    <n v="496"/>
+    <x v="49"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <n v="506"/>
+    <x v="50"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <n v="514"/>
+    <x v="51"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <n v="521"/>
+    <x v="52"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <n v="526"/>
+    <x v="53"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <n v="534"/>
+    <x v="54"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <n v="540"/>
+    <x v="55"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <n v="548"/>
+    <x v="56"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="552"/>
+    <x v="57"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="554"/>
+    <x v="58"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <n v="562"/>
+    <x v="59"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="564"/>
+    <x v="60"/>
+  </r>
+  <r>
+    <n v="16"/>
+    <n v="580"/>
+    <x v="61"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="582"/>
+    <x v="62"/>
+  </r>
+  <r>
+    <n v="21"/>
+    <n v="603"/>
+    <x v="63"/>
+  </r>
+  <r>
+    <n v="11"/>
+    <n v="614"/>
+    <x v="64"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <n v="617"/>
+    <x v="65"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <n v="622"/>
+    <x v="66"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <n v="627"/>
+    <x v="67"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="628"/>
+    <x v="68"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="630"/>
+    <x v="69"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="632"/>
+    <x v="70"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="636"/>
+    <x v="71"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="638"/>
+    <x v="72"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <n v="643"/>
+    <x v="73"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <n v="646"/>
+    <x v="74"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="647"/>
+    <x v="75"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="649"/>
+    <x v="76"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="650"/>
+    <x v="77"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <n v="653"/>
+    <x v="78"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="654"/>
+    <x v="79"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <n v="659"/>
+    <x v="80"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <n v="664"/>
+    <x v="81"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="668"/>
+    <x v="82"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="669"/>
+    <x v="83"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="673"/>
+    <x v="84"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <n v="679"/>
+    <x v="85"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <n v="682"/>
+    <x v="86"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="686"/>
+    <x v="87"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <n v="691"/>
+    <x v="88"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="693"/>
+    <x v="89"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="695"/>
+    <x v="90"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="696"/>
+    <x v="91"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="697"/>
+    <x v="92"/>
+  </r>
+  <r>
+    <n v="11"/>
+    <n v="708"/>
+    <x v="93"/>
+  </r>
+  <r>
+    <n v="15"/>
+    <n v="723"/>
+    <x v="94"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <n v="733"/>
+    <x v="95"/>
+  </r>
+  <r>
+    <n v="11"/>
+    <n v="744"/>
+    <x v="96"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="748"/>
+    <x v="97"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <n v="757"/>
+    <x v="98"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <n v="762"/>
+    <x v="99"/>
+  </r>
+  <r>
+    <n v="17"/>
+    <n v="779"/>
+    <x v="100"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <n v="789"/>
+    <x v="101"/>
+  </r>
+  <r>
+    <n v="12"/>
+    <n v="801"/>
+    <x v="102"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="805"/>
+    <x v="103"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <n v="811"/>
+    <x v="104"/>
+  </r>
+  <r>
+    <n v="19"/>
+    <n v="830"/>
+    <x v="105"/>
+  </r>
+  <r>
+    <n v="12"/>
+    <n v="842"/>
+    <x v="106"/>
+  </r>
+  <r>
+    <n v="31"/>
+    <n v="873"/>
+    <x v="107"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <n v="880"/>
+    <x v="108"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <n v="886"/>
+    <x v="109"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <n v="889"/>
+    <x v="110"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="890"/>
+    <x v="111"/>
+  </r>
+  <r>
+    <n v="14"/>
+    <n v="904"/>
+    <x v="112"/>
+  </r>
+  <r>
+    <n v="25"/>
+    <n v="929"/>
+    <x v="113"/>
+  </r>
+  <r>
+    <n v="14"/>
+    <n v="943"/>
+    <x v="114"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <n v="953"/>
+    <x v="115"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <n v="961"/>
+    <x v="116"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <n v="971"/>
+    <x v="117"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <n v="974"/>
+    <x v="118"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <n v="979"/>
+    <x v="119"/>
+  </r>
+  <r>
+    <n v="11"/>
+    <n v="990"/>
+    <x v="120"/>
+  </r>
+  <r>
+    <n v="32"/>
+    <n v="1022"/>
+    <x v="121"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <n v="1031"/>
+    <x v="122"/>
+  </r>
+  <r>
+    <n v="11"/>
+    <n v="1042"/>
+    <x v="123"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <n v="1049"/>
+    <x v="124"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="1053"/>
+    <x v="125"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="1057"/>
+    <x v="126"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="1061"/>
+    <x v="127"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <n v="1066"/>
+    <x v="128"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <n v="1076"/>
+    <x v="129"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="1077"/>
+    <x v="130"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <n v="1086"/>
+    <x v="131"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="1087"/>
+    <x v="132"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <n v="1095"/>
+    <x v="133"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <n v="1103"/>
+    <x v="134"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <n v="1111"/>
+    <x v="135"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <n v="1120"/>
+    <x v="136"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <n v="1128"/>
+    <x v="137"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <n v="1134"/>
+    <x v="138"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="1135"/>
+    <x v="139"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="1136"/>
+    <x v="140"/>
+  </r>
+  <r>
+    <n v="12"/>
+    <n v="1148"/>
+    <x v="141"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <n v="1154"/>
+    <x v="142"/>
+  </r>
+  <r>
+    <n v="15"/>
+    <n v="1169"/>
+    <x v="143"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <n v="1179"/>
+    <x v="144"/>
+  </r>
+  <r>
+    <n v="12"/>
+    <n v="1191"/>
+    <x v="145"/>
+  </r>
+  <r>
+    <n v="18"/>
+    <n v="1209"/>
+    <x v="146"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <n v="1218"/>
+    <x v="147"/>
+  </r>
+  <r>
+    <n v="35"/>
+    <n v="1253"/>
+    <x v="148"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <n v="1261"/>
+    <x v="149"/>
+  </r>
+  <r>
+    <n v="11"/>
+    <n v="1272"/>
+    <x v="150"/>
+  </r>
+  <r>
+    <n v="12"/>
+    <n v="1284"/>
+    <x v="151"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <n v="1294"/>
+    <x v="152"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="1295"/>
+    <x v="153"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="1299"/>
+    <x v="154"/>
+  </r>
+  <r>
+    <n v="15"/>
+    <n v="1314"/>
+    <x v="155"/>
+  </r>
+  <r>
+    <n v="15"/>
+    <n v="1329"/>
+    <x v="156"/>
+  </r>
+  <r>
+    <n v="13"/>
+    <n v="1342"/>
+    <x v="157"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <n v="1348"/>
+    <x v="158"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <n v="1351"/>
+    <x v="159"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <n v="1356"/>
+    <x v="160"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="1360"/>
+    <x v="161"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <n v="1369"/>
+    <x v="162"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <n v="1374"/>
+    <x v="163"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <n v="1380"/>
+    <x v="164"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="1384"/>
+    <x v="165"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <n v="1387"/>
+    <x v="166"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="1389"/>
+    <x v="167"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="1390"/>
+    <x v="168"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <n v="1399"/>
+    <x v="169"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <n v="1408"/>
+    <x v="170"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <n v="1416"/>
+    <x v="171"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <n v="1422"/>
+    <x v="172"/>
+  </r>
+  <r>
+    <n v="16"/>
+    <n v="1438"/>
+    <x v="173"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <n v="1441"/>
+    <x v="174"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="1443"/>
+    <x v="175"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="1445"/>
+    <x v="176"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <n v="1448"/>
+    <x v="177"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <n v="1454"/>
+    <x v="178"/>
+  </r>
+  <r>
+    <n v="17"/>
+    <n v="1471"/>
+    <x v="179"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <n v="1474"/>
+    <x v="180"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="1476"/>
+    <x v="181"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="1480"/>
+    <x v="182"/>
+  </r>
+  <r>
+    <n v="28"/>
+    <n v="1508"/>
+    <x v="183"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <n v="1513"/>
+    <x v="184"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <n v="1520"/>
+    <x v="185"/>
+  </r>
+  <r>
+    <n v="11"/>
+    <n v="1531"/>
+    <x v="186"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="1533"/>
+    <x v="187"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <n v="1536"/>
+    <x v="188"/>
+  </r>
+  <r>
+    <n v="16"/>
+    <n v="1552"/>
+    <x v="189"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="1556"/>
+    <x v="190"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="1560"/>
+    <x v="191"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <n v="1569"/>
+    <x v="192"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <n v="1574"/>
+    <x v="193"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="1578"/>
+    <x v="194"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="1582"/>
+    <x v="195"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <n v="1590"/>
+    <x v="196"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <n v="1593"/>
+    <x v="197"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <n v="1600"/>
+    <x v="198"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <n v="1606"/>
+    <x v="199"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <n v="1609"/>
+    <x v="200"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="1613"/>
+    <x v="201"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="1615"/>
+    <x v="202"/>
+  </r>
+  <r>
+    <n v="12"/>
+    <n v="1627"/>
+    <x v="203"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <n v="1634"/>
+    <x v="204"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="1635"/>
+    <x v="205"/>
+  </r>
+  <r>
+    <n v="20"/>
+    <n v="1655"/>
+    <x v="206"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <n v="1658"/>
+    <x v="207"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <n v="1663"/>
+    <x v="208"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <n v="1668"/>
+    <x v="209"/>
+  </r>
+  <r>
+    <n v="24"/>
+    <n v="1692"/>
+    <x v="210"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <n v="1700"/>
+    <x v="211"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <n v="1707"/>
+    <x v="212"/>
+  </r>
+  <r>
+    <n v="43"/>
+    <n v="1750"/>
+    <x v="213"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <n v="1755"/>
+    <x v="214"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="1757"/>
+    <x v="215"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <n v="1764"/>
+    <x v="216"/>
+  </r>
+  <r>
+    <n v="18"/>
+    <n v="1782"/>
+    <x v="217"/>
+  </r>
+  <r>
+    <n v="11"/>
+    <n v="1793"/>
+    <x v="218"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <n v="1798"/>
+    <x v="219"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <n v="1805"/>
+    <x v="220"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <n v="1810"/>
+    <x v="221"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="1814"/>
+    <x v="222"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <n v="1819"/>
+    <x v="223"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="1821"/>
+    <x v="224"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <n v="1824"/>
+    <x v="225"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <n v="1833"/>
+    <x v="226"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <n v="1839"/>
+    <x v="227"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <n v="1844"/>
+    <x v="228"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <n v="1847"/>
+    <x v="229"/>
+  </r>
+  <r>
+    <n v="38"/>
+    <n v="1885"/>
+    <x v="230"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <n v="1890"/>
+    <x v="231"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <n v="1896"/>
+    <x v="232"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <n v="1906"/>
+    <x v="233"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <n v="1916"/>
+    <x v="234"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <n v="1922"/>
+    <x v="235"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <n v="1930"/>
+    <x v="236"/>
+  </r>
+  <r>
+    <n v="18"/>
+    <n v="1948"/>
+    <x v="237"/>
+  </r>
+  <r>
+    <n v="42"/>
+    <n v="1990"/>
+    <x v="238"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <n v="2000"/>
+    <x v="239"/>
+  </r>
+  <r>
+    <n v="12"/>
+    <n v="2012"/>
+    <x v="240"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <n v="2020"/>
+    <x v="241"/>
+  </r>
+  <r>
+    <n v="20"/>
+    <n v="2040"/>
+    <x v="242"/>
+  </r>
+  <r>
+    <n v="12"/>
+    <n v="2052"/>
+    <x v="243"/>
+  </r>
+  <r>
+    <n v="19"/>
+    <n v="2071"/>
+    <x v="244"/>
+  </r>
+  <r>
+    <n v="35"/>
+    <n v="2106"/>
+    <x v="245"/>
+  </r>
+  <r>
+    <n v="32"/>
+    <n v="2138"/>
+    <x v="246"/>
+  </r>
+  <r>
+    <n v="24"/>
+    <n v="2162"/>
+    <x v="247"/>
+  </r>
+  <r>
+    <n v="45"/>
+    <n v="2207"/>
+    <x v="248"/>
+  </r>
+  <r>
+    <n v="19"/>
+    <n v="2226"/>
+    <x v="249"/>
+  </r>
+  <r>
+    <n v="15"/>
+    <n v="2241"/>
+    <x v="250"/>
+  </r>
+  <r>
+    <n v="64"/>
+    <n v="2305"/>
+    <x v="251"/>
+  </r>
+  <r>
+    <n v="48"/>
+    <n v="2353"/>
+    <x v="252"/>
+  </r>
+  <r>
+    <n v="69"/>
+    <n v="2422"/>
+    <x v="253"/>
+  </r>
+  <r>
+    <n v="15"/>
+    <n v="2437"/>
+    <x v="254"/>
+  </r>
+  <r>
+    <n v="51"/>
+    <n v="2488"/>
+    <x v="255"/>
+  </r>
+  <r>
+    <n v="84"/>
+    <n v="2572"/>
+    <x v="256"/>
+  </r>
+  <r>
+    <n v="28"/>
+    <n v="2600"/>
+    <x v="257"/>
+  </r>
+  <r>
+    <n v="173"/>
+    <n v="2773"/>
+    <x v="258"/>
+  </r>
+  <r>
+    <n v="50"/>
+    <n v="2823"/>
+    <x v="259"/>
+  </r>
+  <r>
+    <n v="78"/>
+    <n v="2901"/>
+    <x v="260"/>
+  </r>
+  <r>
+    <n v="76"/>
+    <n v="2977"/>
+    <x v="261"/>
+  </r>
+  <r>
+    <n v="128"/>
+    <n v="3105"/>
+    <x v="262"/>
+  </r>
+  <r>
+    <n v="28"/>
+    <n v="3133"/>
+    <x v="263"/>
+  </r>
+  <r>
+    <n v="32"/>
+    <n v="3165"/>
+    <x v="264"/>
+  </r>
+  <r>
+    <n v="165"/>
+    <n v="3330"/>
+    <x v="265"/>
+  </r>
+  <r>
+    <n v="123"/>
+    <n v="3453"/>
+    <x v="266"/>
+  </r>
+  <r>
+    <n v="58"/>
+    <n v="3511"/>
+    <x v="267"/>
+  </r>
+  <r>
+    <n v="82"/>
+    <n v="3593"/>
+    <x v="268"/>
+  </r>
+  <r>
+    <n v="114"/>
+    <n v="3707"/>
+    <x v="269"/>
+  </r>
+  <r>
+    <n v="40"/>
+    <n v="3747"/>
+    <x v="270"/>
+  </r>
+  <r>
+    <n v="61"/>
+    <n v="3808"/>
+    <x v="271"/>
+  </r>
+  <r>
+    <n v="151"/>
+    <n v="3959"/>
+    <x v="272"/>
+  </r>
+  <r>
+    <n v="94"/>
+    <n v="4053"/>
+    <x v="273"/>
+  </r>
+  <r>
+    <n v="88"/>
+    <n v="4141"/>
+    <x v="274"/>
+  </r>
+  <r>
+    <n v="119"/>
+    <n v="4260"/>
+    <x v="275"/>
+  </r>
+  <r>
+    <n v="112"/>
+    <n v="4372"/>
+    <x v="276"/>
+  </r>
+  <r>
+    <n v="66"/>
+    <n v="4438"/>
+    <x v="277"/>
+  </r>
+  <r>
+    <n v="72"/>
+    <n v="4510"/>
+    <x v="278"/>
+  </r>
+  <r>
+    <n v="154"/>
+    <n v="4664"/>
+    <x v="279"/>
+  </r>
+  <r>
+    <n v="80"/>
+    <n v="4744"/>
+    <x v="280"/>
+  </r>
+  <r>
+    <n v="106"/>
+    <n v="4850"/>
+    <x v="281"/>
+  </r>
+  <r>
+    <n v="93"/>
+    <n v="4943"/>
+    <x v="282"/>
+  </r>
+  <r>
+    <n v="19"/>
+    <n v="4962"/>
+    <x v="283"/>
+  </r>
+  <r>
+    <n v="102"/>
+    <n v="5064"/>
+    <x v="284"/>
+  </r>
+  <r>
+    <n v="40"/>
+    <n v="5104"/>
+    <x v="285"/>
+  </r>
+  <r>
+    <n v="105"/>
+    <n v="5209"/>
+    <x v="286"/>
+  </r>
+  <r>
+    <n v="58"/>
+    <n v="5267"/>
+    <x v="287"/>
+  </r>
+  <r>
+    <n v="23"/>
+    <n v="5290"/>
+    <x v="288"/>
+  </r>
+  <r>
+    <n v="59"/>
+    <n v="5349"/>
+    <x v="289"/>
+  </r>
+  <r>
+    <n v="14"/>
+    <n v="5363"/>
+    <x v="290"/>
+  </r>
+  <r>
+    <n v="28"/>
+    <n v="5391"/>
+    <x v="291"/>
+  </r>
+  <r>
+    <n v="36"/>
+    <n v="5427"/>
+    <x v="292"/>
+  </r>
+  <r>
+    <n v="80"/>
+    <n v="5507"/>
+    <x v="293"/>
+  </r>
+  <r>
+    <n v="36"/>
+    <n v="5543"/>
+    <x v="294"/>
+  </r>
+  <r>
+    <n v="29"/>
+    <n v="5572"/>
+    <x v="295"/>
+  </r>
+  <r>
+    <n v="79"/>
+    <n v="5651"/>
+    <x v="296"/>
+  </r>
+  <r>
+    <n v="22"/>
+    <n v="5673"/>
+    <x v="297"/>
+  </r>
+  <r>
+    <n v="24"/>
+    <n v="5697"/>
+    <x v="298"/>
+  </r>
+  <r>
+    <n v="34"/>
+    <n v="5731"/>
+    <x v="299"/>
+  </r>
+  <r>
+    <n v="78"/>
+    <n v="5809"/>
+    <x v="300"/>
+  </r>
+  <r>
+    <n v="43"/>
+    <n v="5852"/>
+    <x v="301"/>
+  </r>
+  <r>
+    <n v="23"/>
+    <n v="5875"/>
+    <x v="302"/>
+  </r>
+  <r>
+    <n v="57"/>
+    <n v="5932"/>
+    <x v="303"/>
+  </r>
+  <r>
+    <n v="26"/>
+    <n v="5958"/>
+    <x v="304"/>
+  </r>
+  <r>
+    <n v="23"/>
+    <n v="5981"/>
+    <x v="305"/>
+  </r>
+  <r>
+    <n v="15"/>
+    <n v="5996"/>
+    <x v="306"/>
+  </r>
+  <r>
+    <n v="47"/>
+    <n v="6043"/>
+    <x v="307"/>
+  </r>
+  <r>
+    <n v="17"/>
+    <n v="6060"/>
+    <x v="308"/>
+  </r>
+  <r>
+    <n v="13"/>
+    <n v="6073"/>
+    <x v="309"/>
+  </r>
+  <r>
+    <n v="32"/>
+    <n v="6105"/>
+    <x v="310"/>
+  </r>
+  <r>
+    <n v="16"/>
+    <n v="6121"/>
+    <x v="311"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <n v="6131"/>
+    <x v="312"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <n v="6141"/>
+    <x v="313"/>
+  </r>
+  <r>
+    <n v="22"/>
+    <n v="6163"/>
+    <x v="314"/>
+  </r>
+  <r>
+    <n v="12"/>
+    <n v="6175"/>
+    <x v="315"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <n v="6183"/>
+    <x v="316"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <n v="6190"/>
+    <x v="317"/>
+  </r>
+  <r>
+    <n v="16"/>
+    <n v="6206"/>
+    <x v="318"/>
+  </r>
+  <r>
+    <n v="19"/>
+    <n v="6225"/>
+    <x v="319"/>
+  </r>
+  <r>
+    <n v="15"/>
+    <n v="6240"/>
+    <x v="320"/>
+  </r>
+  <r>
+    <n v="17"/>
+    <n v="6257"/>
+    <x v="321"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <n v="6267"/>
+    <x v="322"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <n v="6277"/>
+    <x v="323"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <n v="6283"/>
+    <x v="324"/>
+  </r>
+  <r>
+    <n v="12"/>
+    <n v="6295"/>
+    <x v="325"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="6297"/>
+    <x v="326"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6301"/>
+    <x v="327"/>
+  </r>
+  <r>
+    <n v="11"/>
+    <n v="6312"/>
+    <x v="328"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <n v="6319"/>
+    <x v="329"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6323"/>
+    <x v="330"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <n v="6329"/>
+    <x v="331"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="6331"/>
+    <x v="332"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="6332"/>
+    <x v="333"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="6334"/>
+    <x v="334"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="6336"/>
+    <x v="335"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="6338"/>
+    <x v="336"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <n v="6341"/>
+    <x v="337"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="6342"/>
+    <x v="338"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="6343"/>
+    <x v="339"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="6345"/>
+    <x v="340"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6349"/>
+    <x v="341"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="6350"/>
+    <x v="342"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="6352"/>
+    <x v="343"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="6353"/>
+    <x v="344"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="6354"/>
+    <x v="345"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="6356"/>
+    <x v="346"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="6357"/>
+    <x v="347"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="6359"/>
+    <x v="348"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="6361"/>
+    <x v="349"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="6362"/>
+    <x v="350"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="6363"/>
+    <x v="351"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="6364"/>
+    <x v="352"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="6365"/>
+    <x v="353"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="6366"/>
+    <x v="354"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="6367"/>
+    <x v="355"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="6368"/>
+    <x v="356"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="6369"/>
+    <x v="357"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="6370"/>
+    <x v="358"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="6372"/>
+    <x v="359"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="6373"/>
+    <x v="360"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="6374"/>
+    <x v="361"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="6376"/>
+    <x v="362"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="6377"/>
+    <x v="363"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="6378"/>
+    <x v="364"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="6380"/>
+    <x v="365"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="6381"/>
+    <x v="366"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="6382"/>
+    <x v="367"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="6384"/>
+    <x v="368"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="6385"/>
+    <x v="369"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="6386"/>
+    <x v="370"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="6387"/>
+    <x v="371"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="6388"/>
+    <x v="372"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="6389"/>
+    <x v="373"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <n v="6390"/>
+    <x v="374"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <n v="6393"/>
+    <x v="375"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{61557245-6283-4DF5-A42B-EE16A255B64C}" name="PivotTable5" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" numFmtId="14" showAll="0">
+      <items count="377">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="51"/>
+        <item x="52"/>
+        <item x="53"/>
+        <item x="54"/>
+        <item x="55"/>
+        <item x="56"/>
+        <item x="57"/>
+        <item x="58"/>
+        <item x="59"/>
+        <item x="60"/>
+        <item x="61"/>
+        <item x="62"/>
+        <item x="63"/>
+        <item x="64"/>
+        <item x="65"/>
+        <item x="66"/>
+        <item x="67"/>
+        <item x="68"/>
+        <item x="69"/>
+        <item x="70"/>
+        <item x="71"/>
+        <item x="72"/>
+        <item x="73"/>
+        <item x="74"/>
+        <item x="75"/>
+        <item x="76"/>
+        <item x="77"/>
+        <item x="78"/>
+        <item x="79"/>
+        <item x="80"/>
+        <item x="81"/>
+        <item x="82"/>
+        <item x="83"/>
+        <item x="84"/>
+        <item x="85"/>
+        <item x="86"/>
+        <item x="87"/>
+        <item x="88"/>
+        <item x="89"/>
+        <item x="90"/>
+        <item x="91"/>
+        <item x="92"/>
+        <item x="93"/>
+        <item x="94"/>
+        <item x="95"/>
+        <item x="96"/>
+        <item x="97"/>
+        <item x="98"/>
+        <item x="99"/>
+        <item x="100"/>
+        <item x="101"/>
+        <item x="102"/>
+        <item x="103"/>
+        <item x="104"/>
+        <item x="105"/>
+        <item x="106"/>
+        <item x="107"/>
+        <item x="108"/>
+        <item x="109"/>
+        <item x="110"/>
+        <item x="111"/>
+        <item x="112"/>
+        <item x="113"/>
+        <item x="114"/>
+        <item x="115"/>
+        <item x="116"/>
+        <item x="117"/>
+        <item x="118"/>
+        <item x="119"/>
+        <item x="120"/>
+        <item x="121"/>
+        <item x="122"/>
+        <item x="123"/>
+        <item x="124"/>
+        <item x="125"/>
+        <item x="126"/>
+        <item x="127"/>
+        <item x="128"/>
+        <item x="129"/>
+        <item x="130"/>
+        <item x="131"/>
+        <item x="132"/>
+        <item x="133"/>
+        <item x="134"/>
+        <item x="135"/>
+        <item x="136"/>
+        <item x="137"/>
+        <item x="138"/>
+        <item x="139"/>
+        <item x="140"/>
+        <item x="141"/>
+        <item x="142"/>
+        <item x="143"/>
+        <item x="144"/>
+        <item x="145"/>
+        <item x="146"/>
+        <item x="147"/>
+        <item x="148"/>
+        <item x="149"/>
+        <item x="150"/>
+        <item x="151"/>
+        <item x="152"/>
+        <item x="153"/>
+        <item x="154"/>
+        <item x="155"/>
+        <item x="156"/>
+        <item x="157"/>
+        <item x="158"/>
+        <item x="159"/>
+        <item x="160"/>
+        <item x="161"/>
+        <item x="162"/>
+        <item x="163"/>
+        <item x="164"/>
+        <item x="165"/>
+        <item x="166"/>
+        <item x="167"/>
+        <item x="168"/>
+        <item x="169"/>
+        <item x="170"/>
+        <item x="171"/>
+        <item x="172"/>
+        <item x="173"/>
+        <item x="174"/>
+        <item x="175"/>
+        <item x="176"/>
+        <item x="177"/>
+        <item x="178"/>
+        <item x="179"/>
+        <item x="180"/>
+        <item x="181"/>
+        <item x="182"/>
+        <item x="183"/>
+        <item x="184"/>
+        <item x="185"/>
+        <item x="186"/>
+        <item x="187"/>
+        <item x="188"/>
+        <item x="189"/>
+        <item x="190"/>
+        <item x="191"/>
+        <item x="192"/>
+        <item x="193"/>
+        <item x="194"/>
+        <item x="195"/>
+        <item x="196"/>
+        <item x="197"/>
+        <item x="198"/>
+        <item x="199"/>
+        <item x="200"/>
+        <item x="201"/>
+        <item x="202"/>
+        <item x="203"/>
+        <item x="204"/>
+        <item x="205"/>
+        <item x="206"/>
+        <item x="207"/>
+        <item x="208"/>
+        <item x="209"/>
+        <item x="210"/>
+        <item x="211"/>
+        <item x="212"/>
+        <item x="213"/>
+        <item x="214"/>
+        <item x="215"/>
+        <item x="216"/>
+        <item x="217"/>
+        <item x="218"/>
+        <item x="219"/>
+        <item x="220"/>
+        <item x="221"/>
+        <item x="222"/>
+        <item x="223"/>
+        <item x="224"/>
+        <item x="225"/>
+        <item x="226"/>
+        <item x="227"/>
+        <item x="228"/>
+        <item x="229"/>
+        <item x="230"/>
+        <item x="231"/>
+        <item x="232"/>
+        <item x="233"/>
+        <item x="234"/>
+        <item x="235"/>
+        <item x="236"/>
+        <item x="237"/>
+        <item x="238"/>
+        <item x="239"/>
+        <item x="240"/>
+        <item x="241"/>
+        <item x="242"/>
+        <item x="243"/>
+        <item x="244"/>
+        <item x="245"/>
+        <item x="246"/>
+        <item x="247"/>
+        <item x="248"/>
+        <item x="249"/>
+        <item x="250"/>
+        <item x="251"/>
+        <item x="252"/>
+        <item x="253"/>
+        <item x="254"/>
+        <item x="255"/>
+        <item x="256"/>
+        <item x="257"/>
+        <item x="258"/>
+        <item x="259"/>
+        <item x="260"/>
+        <item x="261"/>
+        <item x="262"/>
+        <item x="263"/>
+        <item x="264"/>
+        <item x="265"/>
+        <item x="266"/>
+        <item x="267"/>
+        <item x="268"/>
+        <item x="269"/>
+        <item x="270"/>
+        <item x="271"/>
+        <item x="272"/>
+        <item x="273"/>
+        <item x="274"/>
+        <item x="275"/>
+        <item x="276"/>
+        <item x="277"/>
+        <item x="278"/>
+        <item x="279"/>
+        <item x="280"/>
+        <item x="281"/>
+        <item x="282"/>
+        <item x="283"/>
+        <item x="284"/>
+        <item x="285"/>
+        <item x="286"/>
+        <item x="287"/>
+        <item x="288"/>
+        <item x="289"/>
+        <item x="290"/>
+        <item x="291"/>
+        <item x="292"/>
+        <item x="293"/>
+        <item x="294"/>
+        <item x="295"/>
+        <item x="296"/>
+        <item x="297"/>
+        <item x="298"/>
+        <item x="299"/>
+        <item x="300"/>
+        <item x="301"/>
+        <item x="302"/>
+        <item x="303"/>
+        <item x="304"/>
+        <item x="305"/>
+        <item x="306"/>
+        <item x="307"/>
+        <item x="308"/>
+        <item x="309"/>
+        <item x="310"/>
+        <item x="311"/>
+        <item x="312"/>
+        <item x="313"/>
+        <item x="314"/>
+        <item x="315"/>
+        <item x="316"/>
+        <item x="317"/>
+        <item x="318"/>
+        <item x="319"/>
+        <item x="320"/>
+        <item x="321"/>
+        <item x="322"/>
+        <item x="323"/>
+        <item x="324"/>
+        <item x="325"/>
+        <item x="326"/>
+        <item x="327"/>
+        <item x="328"/>
+        <item x="329"/>
+        <item x="330"/>
+        <item x="331"/>
+        <item x="332"/>
+        <item x="333"/>
+        <item x="334"/>
+        <item x="335"/>
+        <item x="336"/>
+        <item x="337"/>
+        <item x="338"/>
+        <item x="339"/>
+        <item x="340"/>
+        <item x="341"/>
+        <item x="342"/>
+        <item x="343"/>
+        <item x="344"/>
+        <item x="345"/>
+        <item x="346"/>
+        <item x="347"/>
+        <item x="348"/>
+        <item x="349"/>
+        <item x="350"/>
+        <item x="351"/>
+        <item x="352"/>
+        <item x="353"/>
+        <item x="354"/>
+        <item x="355"/>
+        <item x="356"/>
+        <item x="357"/>
+        <item x="358"/>
+        <item x="359"/>
+        <item x="360"/>
+        <item x="361"/>
+        <item x="362"/>
+        <item x="363"/>
+        <item x="364"/>
+        <item x="365"/>
+        <item x="366"/>
+        <item x="367"/>
+        <item x="368"/>
+        <item x="369"/>
+        <item x="370"/>
+        <item x="371"/>
+        <item x="372"/>
+        <item x="373"/>
+        <item x="374"/>
+        <item x="375"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="15">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="6"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="8"/>
+        <item sd="0" x="9"/>
+        <item sd="0" x="10"/>
+        <item sd="0" x="11"/>
+        <item sd="0" x="12"/>
+        <item sd="0" x="13"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item sd="0" x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item sd="0" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="5"/>
+    <field x="4"/>
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of New_cases" fld="0" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6070,11 +8964,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3926422-6703-41F5-BB88-D4446DCC9B4B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05098F39-3EC2-40BB-B08C-FA352CE794D1}">
-  <dimension ref="A1:Y33"/>
+  <dimension ref="A1:Y44"/>
   <sheetViews>
-    <sheetView topLeftCell="B17" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -7583,11 +10490,11 @@
         <v>34</v>
       </c>
       <c r="B28">
-        <f t="shared" ref="B28:Y28" si="3">B6-J17</f>
+        <f>B6-J17</f>
         <v>80</v>
       </c>
       <c r="C28">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="B28:Y28" si="3">C6-K17</f>
         <v>75</v>
       </c>
       <c r="D28">
@@ -8182,6 +11089,92 @@
       <c r="Y33">
         <f t="shared" ref="Y33" si="31">Y11-AG22</f>
         <v>661</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>31</v>
+      </c>
+      <c r="N36">
+        <f>N25/J25</f>
+        <v>1.3846153846153846</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="N37">
+        <f t="shared" ref="N37:N45" si="32">N26/J26</f>
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>33</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="32"/>
+        <v>1.0151515151515151</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>34</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="32"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>35</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="32"/>
+        <v>1.3444976076555024</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>36</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="32"/>
+        <v>1.6579925650557621</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>37</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="32"/>
+        <v>1.3031423290203328</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>38</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="32"/>
+        <v>1.1637816245006658</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>39</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="32"/>
+        <v>1.3268206039076376</v>
       </c>
     </row>
   </sheetData>
@@ -8191,20 +11184,170 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3926422-6703-41F5-BB88-D4446DCC9B4B}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A536F0DC-0CCF-477F-871D-085BAC07AB3E}">
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2">
+        <v>5349</v>
+      </c>
+      <c r="E2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2">
+        <v>5349</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3">
+        <v>101</v>
+      </c>
+      <c r="E3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4">
+        <v>779</v>
+      </c>
+      <c r="E4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5">
+        <v>720</v>
+      </c>
+      <c r="E5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6">
+        <v>3749</v>
+      </c>
+      <c r="E6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6">
+        <v>3749</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7">
+        <v>1044</v>
+      </c>
+      <c r="E7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8">
+        <v>1020</v>
+      </c>
+      <c r="E8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9">
+        <v>24</v>
+      </c>
+      <c r="E9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10">
+        <v>6393</v>
+      </c>
+      <c r="E10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10">
+        <v>6393</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE17"/>
   <sheetViews>
@@ -9295,7 +12438,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C325EDE-41B1-47E7-8DBE-22DBE1D84A13}">
   <dimension ref="A1:Q18"/>
   <sheetViews>
@@ -9929,7 +13072,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U18"/>
   <sheetViews>

</xml_diff>

<commit_message>
updated analysis on FOIA death data
</commit_message>
<xml_diff>
--- a/santa_clara_county/FOIA_data_request_kirsch_analysis.xlsx
+++ b/santa_clara_county/FOIA_data_request_kirsch_analysis.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275C3F76-2BDA-4C43-B910-903927E1A626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B7B556-2766-497D-843F-DCEA831A0FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="67">
   <si>
     <t>age_group</t>
   </si>
@@ -231,6 +231,12 @@
   </si>
   <si>
     <t>NCACM % inncrease of Q1 2021 vs. Q1 2020</t>
+  </si>
+  <si>
+    <t>q4/q1 for covid deaths</t>
+  </si>
+  <si>
+    <t>q1 21 / q1 20 ncacm</t>
   </si>
 </sst>
 </file>
@@ -8978,10 +8984,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05098F39-3EC2-40BB-B08C-FA352CE794D1}">
-  <dimension ref="A1:Y44"/>
+  <dimension ref="A1:Y52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="P47" sqref="P47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -11104,6 +11110,9 @@
         <f>N25/J25</f>
         <v>1.3846153846153846</v>
       </c>
+      <c r="P36" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
@@ -11175,6 +11184,63 @@
       <c r="N44">
         <f t="shared" si="32"/>
         <v>1.3268206039076376</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="M47" t="s">
+        <v>34</v>
+      </c>
+      <c r="N47">
+        <f>N17/M17</f>
+        <v>1.0625</v>
+      </c>
+      <c r="P47" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="M48" t="s">
+        <v>35</v>
+      </c>
+      <c r="N48">
+        <f t="shared" ref="N48:N54" si="33">N18/M18</f>
+        <v>2.4375</v>
+      </c>
+    </row>
+    <row r="49" spans="13:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="M49" t="s">
+        <v>36</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="33"/>
+        <v>1.7391304347826086</v>
+      </c>
+    </row>
+    <row r="50" spans="13:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="M50" t="s">
+        <v>37</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="33"/>
+        <v>1.6440677966101696</v>
+      </c>
+    </row>
+    <row r="51" spans="13:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="M51" t="s">
+        <v>38</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="33"/>
+        <v>1.2590361445783131</v>
+      </c>
+    </row>
+    <row r="52" spans="13:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="M52" t="s">
+        <v>39</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="33"/>
+        <v>1.2167832167832169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated analysis based on baseline NCACM
</commit_message>
<xml_diff>
--- a/santa_clara_county/FOIA_data_request_kirsch_analysis.xlsx
+++ b/santa_clara_county/FOIA_data_request_kirsch_analysis.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B7B556-2766-497D-843F-DCEA831A0FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73AF5776-3E68-4566-BC38-38AE2EA19049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="conclusions" sheetId="5" r:id="rId1"/>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -230,13 +230,13 @@
     <t>local values only copy</t>
   </si>
   <si>
-    <t>NCACM % inncrease of Q1 2021 vs. Q1 2020</t>
-  </si>
-  <si>
     <t>q4/q1 for covid deaths</t>
   </si>
   <si>
-    <t>q1 21 / q1 20 ncacm</t>
+    <t>NCACM % inncrease of Q1 2021 vs. baseline(Q1 of 2018-2020)</t>
+  </si>
+  <si>
+    <t>stunning quarterly increase in COVID deaths after vax rollout</t>
   </si>
 </sst>
 </file>
@@ -8214,7 +8214,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{61557245-6283-4DF5-A42B-EE16A255B64C}" name="PivotTable5" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{61557245-6283-4DF5-A42B-EE16A255B64C}" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField dataField="1" showAll="0"/>
@@ -8975,7 +8975,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8986,18 +8986,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05098F39-3EC2-40BB-B08C-FA352CE794D1}">
   <dimension ref="A1:Y52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="P47" sqref="P47"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -9071,7 +9071,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -9148,7 +9148,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -9225,7 +9225,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -9302,7 +9302,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -9379,7 +9379,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -9456,7 +9456,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -9533,7 +9533,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -9610,7 +9610,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -9687,7 +9687,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -9764,7 +9764,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>52</v>
       </c>
@@ -9841,7 +9841,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -9873,7 +9873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -9899,7 +9899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -9910,7 +9910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -9930,7 +9930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -9950,7 +9950,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -9991,7 +9991,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -10023,7 +10023,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -10070,7 +10070,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -10111,7 +10111,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>51</v>
       </c>
@@ -10188,7 +10188,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -10289,7 +10289,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -10390,7 +10390,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -10491,7 +10491,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -10500,7 +10500,7 @@
         <v>80</v>
       </c>
       <c r="C28">
-        <f t="shared" ref="B28:Y28" si="3">C6-K17</f>
+        <f t="shared" ref="C28:Y28" si="3">C6-K17</f>
         <v>75</v>
       </c>
       <c r="D28">
@@ -10592,7 +10592,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -10693,7 +10693,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -10794,7 +10794,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -10895,7 +10895,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -10996,7 +10996,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -11097,96 +11097,98 @@
         <v>661</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="2" t="s">
-        <v>64</v>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="M35" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" t="s">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="M36" t="s">
         <v>31</v>
       </c>
       <c r="N36">
-        <f>N25/J25</f>
-        <v>1.3846153846153846</v>
-      </c>
-      <c r="P36" t="s">
-        <v>66</v>
+        <f>N25/AVERAGE(B25, F25,J25)</f>
+        <v>1.2272727272727273</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" t="s">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="M37" t="s">
         <v>32</v>
       </c>
       <c r="N37">
-        <f t="shared" ref="N37:N45" si="32">N26/J26</f>
-        <v>1.05</v>
+        <f t="shared" ref="N37:N44" si="32">N26/AVERAGE(B26, F26,J26)</f>
+        <v>1.75</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" t="s">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="M38" t="s">
         <v>33</v>
       </c>
       <c r="N38">
         <f t="shared" si="32"/>
-        <v>1.0151515151515151</v>
+        <v>1.4671532846715329</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" t="s">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="M39" t="s">
         <v>34</v>
       </c>
       <c r="N39">
         <f t="shared" si="32"/>
-        <v>1.5</v>
+        <v>1.4101382488479264</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" t="s">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="M40" t="s">
         <v>35</v>
       </c>
       <c r="N40">
         <f t="shared" si="32"/>
-        <v>1.3444976076555024</v>
+        <v>1.646484375</v>
       </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" t="s">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="M41" t="s">
         <v>36</v>
       </c>
       <c r="N41">
         <f t="shared" si="32"/>
-        <v>1.6579925650557621</v>
+        <v>1.5450346420323324</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" t="s">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="M42" t="s">
         <v>37</v>
       </c>
       <c r="N42">
         <f t="shared" si="32"/>
-        <v>1.3031423290203328</v>
+        <v>1.581899775617053</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" t="s">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="M43" t="s">
         <v>38</v>
       </c>
       <c r="N43">
         <f t="shared" si="32"/>
-        <v>1.1637816245006658</v>
+        <v>1.1875</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" t="s">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="M44" t="s">
         <v>39</v>
       </c>
       <c r="N44">
         <f t="shared" si="32"/>
-        <v>1.3268206039076376</v>
+        <v>1.2732954545454547</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="M46" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="M47" t="s">
         <v>34</v>
       </c>
@@ -11194,20 +11196,20 @@
         <f>N17/M17</f>
         <v>1.0625</v>
       </c>
-      <c r="P47" t="s">
-        <v>65</v>
-      </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="M48" t="s">
         <v>35</v>
       </c>
       <c r="N48">
-        <f t="shared" ref="N48:N54" si="33">N18/M18</f>
+        <f t="shared" ref="N48:N52" si="33">N18/M18</f>
         <v>2.4375</v>
       </c>
+      <c r="P48" t="s">
+        <v>66</v>
+      </c>
     </row>
-    <row r="49" spans="13:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M49" t="s">
         <v>36</v>
       </c>
@@ -11216,7 +11218,7 @@
         <v>1.7391304347826086</v>
       </c>
     </row>
-    <row r="50" spans="13:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M50" t="s">
         <v>37</v>
       </c>
@@ -11225,7 +11227,7 @@
         <v>1.6440677966101696</v>
       </c>
     </row>
-    <row r="51" spans="13:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M51" t="s">
         <v>38</v>
       </c>
@@ -11234,7 +11236,7 @@
         <v>1.2590361445783131</v>
       </c>
     </row>
-    <row r="52" spans="13:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M52" t="s">
         <v>39</v>
       </c>
@@ -11258,9 +11260,9 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>53</v>
       </c>
@@ -11274,7 +11276,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>55</v>
       </c>
@@ -11288,7 +11290,7 @@
         <v>5349</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>56</v>
       </c>
@@ -11302,7 +11304,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>57</v>
       </c>
@@ -11316,7 +11318,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>58</v>
       </c>
@@ -11330,7 +11332,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>59</v>
       </c>
@@ -11344,7 +11346,7 @@
         <v>3749</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>60</v>
       </c>
@@ -11358,7 +11360,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>56</v>
       </c>
@@ -11372,7 +11374,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>57</v>
       </c>
@@ -11386,7 +11388,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>61</v>
       </c>
@@ -11400,7 +11402,7 @@
         <v>6393</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>62</v>
       </c>
@@ -11421,14 +11423,14 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -11523,7 +11525,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -11618,7 +11620,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -11713,7 +11715,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -11808,7 +11810,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -11903,7 +11905,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -11998,7 +12000,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -12093,7 +12095,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -12188,7 +12190,7 @@
         <v>2058</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -12283,7 +12285,7 @@
         <v>3012</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -12378,7 +12380,7 @@
         <v>2587</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -12473,27 +12475,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -12512,14 +12514,14 @@
       <selection activeCell="A3" sqref="A3:Q12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -12572,7 +12574,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -12625,7 +12627,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -12678,7 +12680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -12731,7 +12733,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -12784,7 +12786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -12837,7 +12839,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -12890,7 +12892,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -12943,7 +12945,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -12996,7 +12998,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -13049,7 +13051,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -13102,32 +13104,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>49</v>
       </c>
@@ -13146,14 +13148,14 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -13218,7 +13220,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -13283,7 +13285,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -13348,7 +13350,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -13413,7 +13415,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -13478,7 +13480,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -13543,7 +13545,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -13608,7 +13610,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -13673,7 +13675,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -13738,7 +13740,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -13803,7 +13805,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -13868,32 +13870,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>49</v>
       </c>

</xml_diff>